<commit_message>
Minor update to intro to calculus
</commit_message>
<xml_diff>
--- a/WebsiteCreator/spreadsheets/BinomialDistributions.xlsx
+++ b/WebsiteCreator/spreadsheets/BinomialDistributions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26907"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27816"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/491e2628f664332b/Documents_Charl/Computer_Technical/Programming_GitHub/AustralianSchoolMaths/WebsiteCreator/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="566" documentId="11_F25DC773A252ABDACC10483119D84B8A5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2C2763DB-84C1-4939-8119-62E259471531}"/>
+  <xr:revisionPtr revIDLastSave="586" documentId="11_F25DC773A252ABDACC10483119D84B8A5ADE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BDD19096-6759-43B9-997E-76EC1F96AAB9}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TableOfContents" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Table of contents</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>Has 2 outcomes , 1 for success and 0 for failuire</t>
-  </si>
-  <si>
-    <t>Number of success in n independent Bernoulli trials</t>
   </si>
   <si>
     <t>Distribution</t>
@@ -352,9 +349,6 @@
     <t>E(p̂) = p</t>
   </si>
   <si>
-    <t>VAR(p̂) = p(1-p)/n</t>
-  </si>
-  <si>
     <t>np  (mean of a binomial distribution)</t>
   </si>
   <si>
@@ -377,6 +371,9 @@
   </si>
   <si>
     <t>Totals calculated per table</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -386,8 +383,8 @@
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="#,##0_);\(#,##0\);\-??"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="#,##0_);\(#,##0\);\-??"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -517,7 +514,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -546,14 +543,12 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -683,7 +678,7 @@
               <c:f>BinomialHistogram!NumberOfSuccesses</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -773,66 +768,6 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>36</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>38</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>42</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>43</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>44</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>46</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>47</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>49</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>50</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -842,156 +777,96 @@
               <c:f>BinomialHistogram!Probability</c:f>
               <c:numCache>
                 <c:formatCode>_-* #,##0.00000_-;\-* #,##0.00000_-;_-* "-"??_-;_-@_-</c:formatCode>
-                <c:ptCount val="50"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="0">
-                  <c:v>4.4408920985006262E-14</c:v>
+                  <c:v>2.8979151802318551E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0880185641326534E-12</c:v>
+                  <c:v>1.8008472905726531E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7408297026122455E-11</c:v>
+                  <c:v>7.2033891622906134E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.0454749005693884E-10</c:v>
+                  <c:v>2.0838375790912134E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.8818369085238373E-9</c:v>
+                  <c:v>4.6439808905461323E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.411377681392878E-8</c:v>
+                  <c:v>8.2928230188323779E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.8715168544695189E-8</c:v>
+                  <c:v>0.12185372599100643</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.7684403092773653E-7</c:v>
+                  <c:v>0.15014119809606147</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2252721443294377E-6</c:v>
+                  <c:v>0.15729077895777874</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.1236157917506944E-6</c:v>
+                  <c:v>0.14156170106200083</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.3176784697275239E-5</c:v>
+                  <c:v>0.11030781900935127</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0782455026614457E-4</c:v>
+                  <c:v>7.4851734327774117E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.1517945462411479E-4</c:v>
+                  <c:v>4.4417512678019799E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.329742729351608E-4</c:v>
+                  <c:v>2.3115236189581733E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.9991382550443863E-3</c:v>
+                  <c:v>1.0566965115237364E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4.3731149329095942E-3</c:v>
+                  <c:v>4.2456556266578689E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.7462298658191884E-3</c:v>
+                  <c:v>1.4984666917616009E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.6034754754001852E-2</c:v>
+                  <c:v>4.6381111887859084E-4</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.7005902743582045E-2</c:v>
+                  <c:v>1.2554285924533282E-4</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.1859149252552186E-2</c:v>
+                  <c:v>2.959224539354275E-5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.9798784646503123E-2</c:v>
+                  <c:v>6.039233753784237E-6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.8825670670390452E-2</c:v>
+                  <c:v>1.0588266970920412E-6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.5961686033518873E-2</c:v>
+                  <c:v>1.5783752006340991E-7</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.10795689678770874</c:v>
+                  <c:v>1.9729690007926232E-8</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.11227517265921703</c:v>
+                  <c:v>2.0293395436724135E-9</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.10795689678770874</c:v>
+                  <c:v>1.6725325909388024E-10</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>9.5961686033518873E-2</c:v>
+                  <c:v>1.0619254545643189E-11</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.8825670670390452E-2</c:v>
+                  <c:v>4.8761883117749339E-13</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.9798784646503123E-2</c:v>
+                  <c:v>1.4412379246625421E-14</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.1859149252552186E-2</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>2.7005902743582045E-2</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>1.6034754754001852E-2</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>8.7462298658191884E-3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>4.3731149329095942E-3</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>1.9991382550443863E-3</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>8.329742729351608E-4</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.1517945462411479E-4</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.0782455026614457E-4</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3.3176784697275239E-5</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9.1236157917506944E-6</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2.2252721443294377E-6</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4.7684403092773653E-7</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>8.8715168544695189E-8</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>1.411377681392878E-8</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.8818369085238373E-9</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>2.0454749005693884E-10</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>1.7408297026122455E-11</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>1.0880185641326534E-12</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4.4408920985006262E-14</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>8.8817841970012523E-16</c:v>
+                  <c:v>2.0589113209464887E-16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2615,8 +2490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE454B88-A590-455C-93CF-A67A1DA1FA35}">
   <dimension ref="B2:G26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2633,7 +2508,7 @@
   <sheetData>
     <row r="2" spans="2:7" ht="26" x14ac:dyDescent="0.6">
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.35">
@@ -2646,7 +2521,7 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="29" x14ac:dyDescent="0.35">
@@ -2658,7 +2533,7 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="F7" s="3"/>
     </row>
@@ -2671,14 +2546,14 @@
     </row>
     <row r="9" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -2691,10 +2566,10 @@
     </row>
     <row r="11" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2709,14 +2584,14 @@
     </row>
     <row r="13" spans="2:7" ht="58" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="3"/>
     </row>
@@ -2729,14 +2604,14 @@
     </row>
     <row r="15" spans="2:7" ht="104.5" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="3"/>
     </row>
@@ -2756,14 +2631,14 @@
     </row>
     <row r="18" spans="2:7" ht="116" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -2783,12 +2658,12 @@
     </row>
     <row r="21" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F21" s="3"/>
     </row>
@@ -2801,18 +2676,18 @@
     </row>
     <row r="23" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
@@ -2824,18 +2699,18 @@
     </row>
     <row r="25" spans="2:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>11</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
@@ -2852,7 +2727,7 @@
   <dimension ref="B2:G17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2864,12 +2739,12 @@
   <sheetData>
     <row r="2" spans="2:7" ht="26" x14ac:dyDescent="0.6">
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -2890,7 +2765,7 @@
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -2911,7 +2786,7 @@
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
@@ -2933,8 +2808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DFA3293-B77E-47FF-8323-534F822B45C6}">
   <dimension ref="B1:J65"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2951,7 +2826,7 @@
     </row>
     <row r="2" spans="2:6" ht="26" x14ac:dyDescent="0.6">
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2"/>
     </row>
@@ -2963,18 +2838,18 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="9">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="9">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.35">
@@ -2985,24 +2860,24 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="13">
         <f>SUM(_xlfn.ANCHORARRAY(C16))</f>
-        <v>0.99999999999999911</v>
+        <v>0.99997746065970783</v>
       </c>
       <c r="D9" s="13">
         <f>SUM(_xlfn.ANCHORARRAY(D16))</f>
-        <v>25</v>
+        <v>8.9999999999999858</v>
       </c>
       <c r="E9" s="13">
         <f>SUM(_xlfn.ANCHORARRAY(E16))</f>
-        <v>12.499999999999446</v>
+        <v>6.2981743134364452</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B10" s="15" t="s">
-        <v>39</v>
+      <c r="B10" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="13">
         <v>1</v>
@@ -3011,42 +2886,42 @@
       <c r="E10" s="13"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B11" s="16" t="s">
-        <v>40</v>
+      <c r="B11" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="13"/>
       <c r="D11" s="13">
         <f>C6*C5</f>
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="E11" s="13"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B12" s="16" t="s">
-        <v>41</v>
+      <c r="B12" t="s">
+        <v>39</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="13"/>
       <c r="E12" s="13">
         <f>C6*C5*(1-C5)</f>
-        <v>12.5</v>
+        <v>6.3</v>
       </c>
     </row>
     <row r="13" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="17">
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="15">
         <f>C9-SUM(C10:C12)</f>
-        <v>-8.8817841970012523E-16</v>
-      </c>
-      <c r="D13" s="17">
+        <v>-2.2539340292171417E-5</v>
+      </c>
+      <c r="D13" s="15">
         <f t="shared" ref="D13:E13" si="0">D9-SUM(D10:D12)</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="17">
+        <v>-1.4210854715202004E-14</v>
+      </c>
+      <c r="E13" s="15">
         <f t="shared" si="0"/>
-        <v>-5.5422333389287814E-13</v>
+        <v>-1.8256865635546404E-3</v>
       </c>
     </row>
     <row r="14" spans="2:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -3055,381 +2930,381 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B15" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>33</v>
-      </c>
       <c r="D15" s="12" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B16" cm="1">
-        <f t="array" ref="B16:B65">_xlfn.SEQUENCE(C6)</f>
+        <f t="array" ref="B16:B45">_xlfn.SEQUENCE(C6)</f>
         <v>1</v>
       </c>
       <c r="C16" s="6" cm="1">
-        <f t="array" ref="C16:C65">COMBIN($C$6,_xlfn.ANCHORARRAY(B16)) * $C$5^_xlfn.ANCHORARRAY(B16) * (1-$C$5)^($C$6-_xlfn.ANCHORARRAY(B16))</f>
-        <v>4.4408920985006262E-14</v>
+        <f t="array" ref="C16:C45">COMBIN($C$6,_xlfn.ANCHORARRAY(B16)) * $C$5^_xlfn.ANCHORARRAY(B16) * (1-$C$5)^($C$6-_xlfn.ANCHORARRAY(B16))</f>
+        <v>2.8979151802318551E-4</v>
       </c>
       <c r="D16" s="14" cm="1">
-        <f t="array" ref="D16:D65">_xlfn.ANCHORARRAY(B16)*_xlfn.ANCHORARRAY(C16)</f>
-        <v>4.4408920985006262E-14</v>
+        <f t="array" ref="D16:D45">_xlfn.ANCHORARRAY(B16)*_xlfn.ANCHORARRAY(C16)</f>
+        <v>2.8979151802318551E-4</v>
       </c>
       <c r="E16" s="11" cm="1">
-        <f t="array" ref="E16:E65">(_xlfn.ANCHORARRAY(B16)-$D$9)^2*_xlfn.ANCHORARRAY(C16)</f>
-        <v>2.5579538487363607E-11</v>
-      </c>
-      <c r="F16" s="19"/>
+        <f t="array" ref="E16:E45">(_xlfn.ANCHORARRAY(B16)-$D$9)^2*_xlfn.ANCHORARRAY(C16)</f>
+        <v>1.8546657153483807E-2</v>
+      </c>
+      <c r="F16" s="17"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" s="6">
-        <v>1.0880185641326534E-12</v>
+        <v>1.8008472905726531E-3</v>
       </c>
       <c r="D17" s="14">
-        <v>2.1760371282653068E-12</v>
+        <v>3.6016945811453063E-3</v>
       </c>
       <c r="E17" s="11">
-        <v>5.7556182042617365E-10</v>
-      </c>
-      <c r="F17" s="19"/>
+        <v>8.8241517238059647E-2</v>
+      </c>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>3</v>
       </c>
       <c r="C18" s="6">
-        <v>1.7408297026122455E-11</v>
+        <v>7.2033891622906134E-3</v>
       </c>
       <c r="D18" s="14">
-        <v>5.2224891078367364E-11</v>
+        <v>2.1610167486871841E-2</v>
       </c>
       <c r="E18" s="11">
-        <v>8.425615760643268E-9</v>
-      </c>
-      <c r="F18" s="19"/>
+        <v>0.25932200984246084</v>
+      </c>
+      <c r="F18" s="17"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>4</v>
       </c>
       <c r="C19" s="6">
-        <v>2.0454749005693884E-10</v>
+        <v>2.0838375790912134E-2</v>
       </c>
       <c r="D19" s="14">
-        <v>8.1818996022775536E-10</v>
+        <v>8.3353503163648535E-2</v>
       </c>
       <c r="E19" s="11">
-        <v>9.0205443115110029E-8</v>
-      </c>
-      <c r="F19" s="19"/>
+        <v>0.5209593947728004</v>
+      </c>
+      <c r="F19" s="17"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>5</v>
       </c>
       <c r="C20" s="6">
-        <v>1.8818369085238373E-9</v>
+        <v>4.6439808905461323E-2</v>
       </c>
       <c r="D20" s="14">
-        <v>9.4091845426191867E-9</v>
+        <v>0.23219904452730661</v>
       </c>
       <c r="E20" s="11">
-        <v>7.5273476340953493E-7</v>
-      </c>
-      <c r="F20" s="19"/>
+        <v>0.74303694248737584</v>
+      </c>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>6</v>
       </c>
       <c r="C21" s="6">
-        <v>1.411377681392878E-8</v>
+        <v>8.2928230188323779E-2</v>
       </c>
       <c r="D21" s="14">
-        <v>8.468266088357268E-8</v>
+        <v>0.49756938112994265</v>
       </c>
       <c r="E21" s="11">
-        <v>5.0950734298282896E-6</v>
-      </c>
-      <c r="F21" s="19"/>
+        <v>0.74635407169490697</v>
+      </c>
+      <c r="F21" s="17"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>7</v>
       </c>
       <c r="C22" s="6">
-        <v>8.8715168544695189E-8</v>
+        <v>0.12185372599100643</v>
       </c>
       <c r="D22" s="14">
-        <v>6.2100617981286632E-7</v>
+        <v>0.85297608193704499</v>
       </c>
       <c r="E22" s="11">
-        <v>2.8743714608481241E-5</v>
-      </c>
-      <c r="F22" s="19"/>
+        <v>0.48741490396401876</v>
+      </c>
+      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>8</v>
       </c>
       <c r="C23" s="6">
-        <v>4.7684403092773653E-7</v>
+        <v>0.15014119809606147</v>
       </c>
       <c r="D23" s="14">
-        <v>3.8147522474218923E-6</v>
+        <v>1.2011295847684917</v>
       </c>
       <c r="E23" s="11">
-        <v>1.3780792493811586E-4</v>
-      </c>
-      <c r="F23" s="19"/>
+        <v>0.15014119809605719</v>
+      </c>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>9</v>
       </c>
       <c r="C24" s="6">
-        <v>2.2252721443294377E-6</v>
+        <v>0.15729077895777874</v>
       </c>
       <c r="D24" s="14">
-        <v>2.0027449298964939E-5</v>
+        <v>1.4156170106200086</v>
       </c>
       <c r="E24" s="11">
-        <v>5.6966966894833604E-4</v>
-      </c>
-      <c r="F24" s="19"/>
+        <v>3.1764619845517161E-29</v>
+      </c>
+      <c r="F24" s="17"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>10</v>
       </c>
       <c r="C25" s="6">
-        <v>9.1236157917506944E-6</v>
+        <v>0.14156170106200083</v>
       </c>
       <c r="D25" s="14">
-        <v>9.1236157917506944E-5</v>
+        <v>1.4156170106200083</v>
       </c>
       <c r="E25" s="11">
-        <v>2.0528135531439062E-3</v>
-      </c>
-      <c r="F25" s="19"/>
+        <v>0.14156170106200486</v>
+      </c>
+      <c r="F25" s="17"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>11</v>
       </c>
       <c r="C26" s="6">
-        <v>3.3176784697275239E-5</v>
+        <v>0.11030781900935127</v>
       </c>
       <c r="D26" s="14">
-        <v>3.6494463167002761E-4</v>
+        <v>1.2133860091028641</v>
       </c>
       <c r="E26" s="11">
-        <v>6.5026498006659468E-3</v>
-      </c>
-      <c r="F26" s="19"/>
+        <v>0.44123127603741136</v>
+      </c>
+      <c r="F26" s="17"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>12</v>
       </c>
       <c r="C27" s="6">
-        <v>1.0782455026614457E-4</v>
+        <v>7.4851734327774117E-2</v>
       </c>
       <c r="D27" s="14">
-        <v>1.2938946031937348E-3</v>
+        <v>0.8982208119332894</v>
       </c>
       <c r="E27" s="11">
-        <v>1.8222348994978432E-2</v>
-      </c>
-      <c r="F27" s="19"/>
+        <v>0.6736656089499734</v>
+      </c>
+      <c r="F27" s="17"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>13</v>
       </c>
       <c r="C28" s="6">
-        <v>3.1517945462411479E-4</v>
+        <v>4.4417512678019799E-2</v>
       </c>
       <c r="D28" s="14">
-        <v>4.0973329101134919E-3</v>
+        <v>0.57742766481425734</v>
       </c>
       <c r="E28" s="11">
-        <v>4.5385841465872531E-2</v>
-      </c>
-      <c r="F28" s="19"/>
+        <v>0.71068020284832178</v>
+      </c>
+      <c r="F28" s="17"/>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>14</v>
       </c>
       <c r="C29" s="6">
-        <v>8.329742729351608E-4</v>
+        <v>2.3115236189581733E-2</v>
       </c>
       <c r="D29" s="14">
-        <v>1.1661639821092251E-2</v>
+        <v>0.32361330665414428</v>
       </c>
       <c r="E29" s="11">
-        <v>0.10078988702515446</v>
-      </c>
-      <c r="F29" s="19"/>
+        <v>0.57788090473954656</v>
+      </c>
+      <c r="F29" s="17"/>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>15</v>
       </c>
       <c r="C30" s="6">
-        <v>1.9991382550443863E-3</v>
+        <v>1.0566965115237364E-2</v>
       </c>
       <c r="D30" s="14">
-        <v>2.9987073825665796E-2</v>
+        <v>0.15850447672856047</v>
       </c>
       <c r="E30" s="11">
-        <v>0.19991382550443865</v>
-      </c>
-      <c r="F30" s="19"/>
+        <v>0.38041074414854692</v>
+      </c>
+      <c r="F30" s="17"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>16</v>
       </c>
       <c r="C31" s="6">
-        <v>4.3731149329095942E-3</v>
+        <v>4.2456556266578689E-3</v>
       </c>
       <c r="D31" s="14">
-        <v>6.9969838926553507E-2</v>
+        <v>6.7930490026525903E-2</v>
       </c>
       <c r="E31" s="11">
-        <v>0.35422230956567713</v>
-      </c>
-      <c r="F31" s="19"/>
+        <v>0.20803712570623642</v>
+      </c>
+      <c r="F31" s="17"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>17</v>
       </c>
       <c r="C32" s="6">
-        <v>8.7462298658191884E-3</v>
+        <v>1.4984666917616009E-3</v>
       </c>
       <c r="D32" s="14">
-        <v>0.1486859077189262</v>
+        <v>2.5473933759947213E-2</v>
       </c>
       <c r="E32" s="11">
-        <v>0.55975871141242806</v>
-      </c>
-      <c r="F32" s="19"/>
+        <v>9.5901868272742802E-2</v>
+      </c>
+      <c r="F32" s="17"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>18</v>
       </c>
       <c r="C33" s="6">
-        <v>1.6034754754001852E-2</v>
+        <v>4.6381111887859084E-4</v>
       </c>
       <c r="D33" s="14">
-        <v>0.28862558557203333</v>
+        <v>8.348600139814635E-3</v>
       </c>
       <c r="E33" s="11">
-        <v>0.78570298294609076</v>
-      </c>
-      <c r="F33" s="19"/>
+        <v>3.756870062916598E-2</v>
+      </c>
+      <c r="F33" s="17"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>19</v>
       </c>
       <c r="C34" s="6">
-        <v>2.7005902743582045E-2</v>
+        <v>1.2554285924533282E-4</v>
       </c>
       <c r="D34" s="14">
-        <v>0.51311215212805883</v>
+        <v>2.3853143256613234E-3</v>
       </c>
       <c r="E34" s="11">
-        <v>0.97221249876895366</v>
-      </c>
-      <c r="F34" s="19"/>
+        <v>1.2554285924533318E-2</v>
+      </c>
+      <c r="F34" s="17"/>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>20</v>
       </c>
       <c r="C35" s="6">
-        <v>4.1859149252552186E-2</v>
+        <v>2.959224539354275E-5</v>
       </c>
       <c r="D35" s="14">
-        <v>0.83718298505104372</v>
+        <v>5.91844907870855E-4</v>
       </c>
       <c r="E35" s="11">
-        <v>1.0464787313138046</v>
-      </c>
-      <c r="F35" s="19"/>
+        <v>3.5806616926186822E-3</v>
+      </c>
+      <c r="F35" s="17"/>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>21</v>
       </c>
       <c r="C36" s="6">
-        <v>5.9798784646503123E-2</v>
+        <v>6.039233753784237E-6</v>
       </c>
       <c r="D36" s="14">
-        <v>1.2557744775765656</v>
+        <v>1.2682390882946899E-4</v>
       </c>
       <c r="E36" s="11">
-        <v>0.95678055434404996</v>
-      </c>
-      <c r="F36" s="19"/>
+        <v>8.6964966054493213E-4</v>
+      </c>
+      <c r="F36" s="17"/>
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>22</v>
       </c>
       <c r="C37" s="6">
-        <v>7.8825670670390452E-2</v>
+        <v>1.0588266970920412E-6</v>
       </c>
       <c r="D37" s="14">
-        <v>1.7341647547485899</v>
+        <v>2.3294187336024908E-5</v>
       </c>
       <c r="E37" s="11">
-        <v>0.7094310360335141</v>
-      </c>
-      <c r="F37" s="19"/>
+        <v>1.7894171180855536E-4</v>
+      </c>
+      <c r="F37" s="17"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>23</v>
       </c>
       <c r="C38" s="6">
-        <v>9.5961686033518873E-2</v>
+        <v>1.5783752006340991E-7</v>
       </c>
       <c r="D38" s="14">
-        <v>2.2071187787709339</v>
+        <v>3.6302629614584278E-6</v>
       </c>
       <c r="E38" s="11">
-        <v>0.38384674413407549</v>
-      </c>
-      <c r="F38" s="19"/>
+        <v>3.0936153932428405E-5</v>
+      </c>
+      <c r="F38" s="17"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>24</v>
       </c>
       <c r="C39" s="6">
-        <v>0.10795689678770874</v>
+        <v>1.9729690007926232E-8</v>
       </c>
       <c r="D39" s="14">
-        <v>2.5909655229050097</v>
+        <v>4.7351256019022955E-7</v>
       </c>
       <c r="E39" s="11">
-        <v>0.10795689678770874</v>
-      </c>
-      <c r="F39" s="19"/>
+        <v>4.4391802517834109E-6</v>
+      </c>
+      <c r="F39" s="17"/>
       <c r="H39" s="7"/>
       <c r="J39" s="10" t="str" cm="1">
         <f t="array" ref="J39">_xlfn.SWITCH(
@@ -3439,7 +3314,7 @@
     C5&gt;0.5, "p &gt; 0.5 therefore graph is negatively skewed",
     "TBA"
 )</f>
-        <v>p = 0.5 therefore graph is symmetrical</v>
+        <v>p &lt; 0.5 therefore graph is positively skewed</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.35">
@@ -3447,15 +3322,15 @@
         <v>25</v>
       </c>
       <c r="C40" s="6">
-        <v>0.11227517265921703</v>
+        <v>2.0293395436724135E-9</v>
       </c>
       <c r="D40" s="14">
-        <v>2.8068793164804258</v>
+        <v>5.0733488591810338E-8</v>
       </c>
       <c r="E40" s="11">
-        <v>0</v>
-      </c>
-      <c r="F40" s="19"/>
+        <v>5.195109231801388E-7</v>
+      </c>
+      <c r="F40" s="17"/>
       <c r="H40" s="7"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.35">
@@ -3463,47 +3338,47 @@
         <v>26</v>
       </c>
       <c r="C41" s="6">
-        <v>0.10795689678770874</v>
+        <v>1.6725325909388024E-10</v>
       </c>
       <c r="D41" s="14">
-        <v>2.8068793164804271</v>
+        <v>4.3485847364408858E-9</v>
       </c>
       <c r="E41" s="11">
-        <v>0.10795689678770874</v>
-      </c>
-      <c r="F41" s="19"/>
-      <c r="H41" s="18"/>
+        <v>4.8336191878131466E-8</v>
+      </c>
+      <c r="F41" s="17"/>
+      <c r="H41" s="16"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>27</v>
       </c>
       <c r="C42" s="6">
-        <v>9.5961686033518873E-2</v>
+        <v>1.0619254545643189E-11</v>
       </c>
       <c r="D42" s="14">
-        <v>2.5909655229050097</v>
+        <v>2.8671987273236612E-10</v>
       </c>
       <c r="E42" s="11">
-        <v>0.38384674413407549</v>
-      </c>
-      <c r="F42" s="19"/>
-      <c r="H42" s="18"/>
+        <v>3.4406384727883984E-9</v>
+      </c>
+      <c r="F42" s="17"/>
+      <c r="H42" s="16"/>
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>28</v>
       </c>
       <c r="C43" s="6">
-        <v>7.8825670670390452E-2</v>
+        <v>4.8761883117749339E-13</v>
       </c>
       <c r="D43" s="14">
-        <v>2.2071187787709325</v>
+        <v>1.3653327272969814E-11</v>
       </c>
       <c r="E43" s="11">
-        <v>0.7094310360335141</v>
-      </c>
-      <c r="F43" s="19"/>
+        <v>1.7603039805507539E-10</v>
+      </c>
+      <c r="F43" s="17"/>
       <c r="H43" s="7"/>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.35">
@@ -3511,333 +3386,133 @@
         <v>29</v>
       </c>
       <c r="C44" s="6">
-        <v>5.9798784646503123E-2</v>
+        <v>1.4412379246625421E-14</v>
       </c>
       <c r="D44" s="14">
-        <v>1.7341647547485906</v>
+        <v>4.1795899815213722E-13</v>
       </c>
       <c r="E44" s="11">
-        <v>0.95678055434404996</v>
-      </c>
-      <c r="F44" s="19"/>
+        <v>5.7649516986501771E-12</v>
+      </c>
+      <c r="F44" s="17"/>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45">
         <v>30</v>
       </c>
       <c r="C45" s="6">
-        <v>4.1859149252552186E-2</v>
+        <v>2.0589113209464887E-16</v>
       </c>
       <c r="D45" s="14">
-        <v>1.2557744775765656</v>
+        <v>6.1767339628394659E-15</v>
       </c>
       <c r="E45" s="11">
-        <v>1.0464787313138046</v>
-      </c>
-      <c r="F45" s="19"/>
+        <v>9.079798925374027E-14</v>
+      </c>
+      <c r="F45" s="17"/>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B46">
-        <v>31</v>
-      </c>
-      <c r="C46" s="6">
-        <v>2.7005902743582045E-2</v>
-      </c>
-      <c r="D46" s="14">
-        <v>0.83718298505104338</v>
-      </c>
-      <c r="E46" s="11">
-        <v>0.97221249876895366</v>
-      </c>
-      <c r="F46" s="19"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="17"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B47">
-        <v>32</v>
-      </c>
-      <c r="C47" s="6">
-        <v>1.6034754754001852E-2</v>
-      </c>
-      <c r="D47" s="14">
-        <v>0.51311215212805927</v>
-      </c>
-      <c r="E47" s="11">
-        <v>0.78570298294609076</v>
-      </c>
-      <c r="F47" s="19"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="17"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B48">
-        <v>33</v>
-      </c>
-      <c r="C48" s="6">
-        <v>8.7462298658191884E-3</v>
-      </c>
-      <c r="D48" s="14">
-        <v>0.28862558557203322</v>
-      </c>
-      <c r="E48" s="11">
-        <v>0.55975871141242806</v>
-      </c>
-      <c r="F48" s="19"/>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B49">
-        <v>34</v>
-      </c>
-      <c r="C49" s="6">
-        <v>4.3731149329095942E-3</v>
-      </c>
-      <c r="D49" s="14">
-        <v>0.1486859077189262</v>
-      </c>
-      <c r="E49" s="11">
-        <v>0.35422230956567713</v>
-      </c>
-      <c r="F49" s="19"/>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B50">
-        <v>35</v>
-      </c>
-      <c r="C50" s="6">
-        <v>1.9991382550443863E-3</v>
-      </c>
-      <c r="D50" s="14">
-        <v>6.9969838926553521E-2</v>
-      </c>
-      <c r="E50" s="11">
-        <v>0.19991382550443865</v>
-      </c>
-      <c r="F50" s="19"/>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B51">
-        <v>36</v>
-      </c>
-      <c r="C51" s="6">
-        <v>8.329742729351608E-4</v>
-      </c>
-      <c r="D51" s="14">
-        <v>2.9987073825665789E-2</v>
-      </c>
-      <c r="E51" s="11">
-        <v>0.10078988702515446</v>
-      </c>
-      <c r="F51" s="19"/>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B52">
-        <v>37</v>
-      </c>
-      <c r="C52" s="6">
-        <v>3.1517945462411479E-4</v>
-      </c>
-      <c r="D52" s="14">
-        <v>1.1661639821092248E-2</v>
-      </c>
-      <c r="E52" s="11">
-        <v>4.5385841465872531E-2</v>
-      </c>
-      <c r="F52" s="19"/>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B53">
-        <v>38</v>
-      </c>
-      <c r="C53" s="6">
-        <v>1.0782455026614457E-4</v>
-      </c>
-      <c r="D53" s="14">
-        <v>4.0973329101134937E-3</v>
-      </c>
-      <c r="E53" s="11">
-        <v>1.8222348994978432E-2</v>
-      </c>
-      <c r="F53" s="19"/>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B54">
-        <v>39</v>
-      </c>
-      <c r="C54" s="6">
-        <v>3.3176784697275239E-5</v>
-      </c>
-      <c r="D54" s="14">
-        <v>1.2938946031937344E-3</v>
-      </c>
-      <c r="E54" s="11">
-        <v>6.5026498006659468E-3</v>
-      </c>
-      <c r="F54" s="19"/>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B55">
-        <v>40</v>
-      </c>
-      <c r="C55" s="6">
-        <v>9.1236157917506944E-6</v>
-      </c>
-      <c r="D55" s="14">
-        <v>3.6494463167002777E-4</v>
-      </c>
-      <c r="E55" s="11">
-        <v>2.0528135531439062E-3</v>
-      </c>
-      <c r="F55" s="19"/>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B56">
-        <v>41</v>
-      </c>
-      <c r="C56" s="6">
-        <v>2.2252721443294377E-6</v>
-      </c>
-      <c r="D56" s="14">
-        <v>9.1236157917506944E-5</v>
-      </c>
-      <c r="E56" s="11">
-        <v>5.6966966894833604E-4</v>
-      </c>
-      <c r="F56" s="19"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B57">
-        <v>42</v>
-      </c>
-      <c r="C57" s="6">
-        <v>4.7684403092773653E-7</v>
-      </c>
-      <c r="D57" s="14">
-        <v>2.0027449298964935E-5</v>
-      </c>
-      <c r="E57" s="11">
-        <v>1.3780792493811586E-4</v>
-      </c>
-      <c r="F57" s="19"/>
-    </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B58">
-        <v>43</v>
-      </c>
-      <c r="C58" s="6">
-        <v>8.8715168544695189E-8</v>
-      </c>
-      <c r="D58" s="14">
-        <v>3.8147522474218931E-6</v>
-      </c>
-      <c r="E58" s="11">
-        <v>2.8743714608481241E-5</v>
-      </c>
-      <c r="F58" s="19"/>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B59">
-        <v>44</v>
-      </c>
-      <c r="C59" s="6">
-        <v>1.411377681392878E-8</v>
-      </c>
-      <c r="D59" s="14">
-        <v>6.2100617981286632E-7</v>
-      </c>
-      <c r="E59" s="11">
-        <v>5.0950734298282896E-6</v>
-      </c>
-      <c r="F59" s="19"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B60">
-        <v>45</v>
-      </c>
-      <c r="C60" s="6">
-        <v>1.8818369085238373E-9</v>
-      </c>
-      <c r="D60" s="14">
-        <v>8.468266088357268E-8</v>
-      </c>
-      <c r="E60" s="11">
-        <v>7.5273476340953493E-7</v>
-      </c>
-      <c r="F60" s="19"/>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B61">
-        <v>46</v>
-      </c>
-      <c r="C61" s="6">
-        <v>2.0454749005693884E-10</v>
-      </c>
-      <c r="D61" s="14">
-        <v>9.4091845426191867E-9</v>
-      </c>
-      <c r="E61" s="11">
-        <v>9.0205443115110029E-8</v>
-      </c>
-      <c r="F61" s="19"/>
-    </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B62">
-        <v>47</v>
-      </c>
-      <c r="C62" s="6">
-        <v>1.7408297026122455E-11</v>
-      </c>
-      <c r="D62" s="14">
-        <v>8.1818996022775536E-10</v>
-      </c>
-      <c r="E62" s="11">
-        <v>8.425615760643268E-9</v>
-      </c>
-      <c r="F62" s="19"/>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B63">
-        <v>48</v>
-      </c>
-      <c r="C63" s="6">
-        <v>1.0880185641326534E-12</v>
-      </c>
-      <c r="D63" s="14">
-        <v>5.2224891078367364E-11</v>
-      </c>
-      <c r="E63" s="11">
-        <v>5.7556182042617365E-10</v>
-      </c>
-      <c r="F63" s="19"/>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B64">
-        <v>49</v>
-      </c>
-      <c r="C64" s="6">
-        <v>4.4408920985006262E-14</v>
-      </c>
-      <c r="D64" s="14">
-        <v>2.1760371282653068E-12</v>
-      </c>
-      <c r="E64" s="11">
-        <v>2.5579538487363607E-11</v>
-      </c>
-      <c r="F64" s="19"/>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B65">
-        <v>50</v>
-      </c>
-      <c r="C65" s="6">
-        <v>8.8817841970012523E-16</v>
-      </c>
-      <c r="D65" s="14">
-        <v>4.4408920985006262E-14</v>
-      </c>
-      <c r="E65" s="11">
-        <v>5.5511151231257827E-13</v>
-      </c>
-      <c r="F65" s="19"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="17"/>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D49" s="14"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="17"/>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D50" s="14"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="17"/>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D51" s="14"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="17"/>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D52" s="14"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="17"/>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D53" s="14"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="17"/>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D54" s="14"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="17"/>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D55" s="14"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="17"/>
+    </row>
+    <row r="56" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D56" s="14"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="17"/>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D57" s="14"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="17"/>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D58" s="14"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="17"/>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D59" s="14"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="17"/>
+    </row>
+    <row r="60" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D60" s="14"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="17"/>
+    </row>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D61" s="14"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="17"/>
+    </row>
+    <row r="62" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D62" s="14"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="17"/>
+    </row>
+    <row r="63" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D63" s="14"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="17"/>
+    </row>
+    <row r="64" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D64" s="14"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="17"/>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D65" s="14"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="17"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5" xr:uid="{780A1BAA-64DA-4840-B8AE-50D5F17909CC}">
       <formula1>"0.1,0.2,0.3,0.4,0.5,0.6,0.7,0.8,0.9"</formula1>
     </dataValidation>

</xml_diff>